<commit_message>
Pulp and Paper sector overhaul
Joseph has redone the sector. Steam now central to the modelling.
CHP still a bit problematic.
</commit_message>
<xml_diff>
--- a/suppxls/Scen_UC_IND_IPP.xlsx
+++ b/suppxls/Scen_UC_IND_IPP.xlsx
@@ -8,21 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9786C1F-36F8-4689-92E8-BBFB0CA5C6BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34B21B6-6CE7-4100-871A-495EF64EDDC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35925" yWindow="3645" windowWidth="17280" windowHeight="8970" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UCT1" sheetId="2" r:id="rId1"/>
     <sheet name="UCT2" sheetId="3" r:id="rId2"/>
-    <sheet name="UCT4" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="43">
   <si>
     <t>UC - Each Region/Period</t>
   </si>
@@ -150,52 +149,7 @@
     <t>Biomass consumed for piulping</t>
   </si>
   <si>
-    <t>UCACT_IPP_CHP</t>
-  </si>
-  <si>
-    <t>Set max fossil fuel (FF) share to renewable (RE) fuel utilisation ratio</t>
-  </si>
-  <si>
-    <t>Dissolving pulp</t>
-  </si>
-  <si>
-    <t>Chemical pulping</t>
-  </si>
-  <si>
-    <t>IPPCHE_N</t>
-  </si>
-  <si>
-    <t>IPPDIS_E</t>
-  </si>
-  <si>
-    <t>LO</t>
-  </si>
-  <si>
-    <t>Market shares</t>
-  </si>
-  <si>
-    <t>Mechanical Pulp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chemical Pulp </t>
-  </si>
-  <si>
-    <t>Semi-chemical Pulp</t>
-  </si>
-  <si>
-    <t>Dissolving wood Pulp</t>
-  </si>
-  <si>
-    <t>Total Pulp</t>
-  </si>
-  <si>
-    <t>Min ratio of DIS to Che pulping</t>
-  </si>
-  <si>
-    <t>IPPDIS-N, IPPDIS-E</t>
-  </si>
-  <si>
-    <t>IPPCHE-N, IPPCHE-E</t>
+    <t>IPPSTMBIO-E</t>
   </si>
 </sst>
 </file>
@@ -209,7 +163,7 @@
     <numFmt numFmtId="166" formatCode="[$£-809]#,##0.000;[Red]&quot;-&quot;[$£-809]#,##0.000"/>
     <numFmt numFmtId="167" formatCode="[$£-809]#,##0.00;[Red]&quot;-&quot;[$£-809]#,##0.00"/>
   </numFmts>
-  <fonts count="39" x14ac:knownFonts="1">
+  <fonts count="38" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -352,6 +306,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -440,13 +395,6 @@
       <color theme="6" tint="-0.24994659260841701"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -574,7 +522,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -630,21 +578,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="178">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -829,11 +762,11 @@
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="167" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="4" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="4" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -844,7 +777,7 @@
     <xf numFmtId="167" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="167" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -865,9 +798,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="36" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="178">
     <cellStyle name="20% - Accent1 2" xfId="17" xr:uid="{03071494-95FB-4D44-BFD8-23D5C5460AB0}"/>
@@ -1380,7 +1310,7 @@
   <dimension ref="B1:S18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1739,7 +1669,7 @@
   <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1914,7 +1844,7 @@
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="13" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1947,7 +1877,7 @@
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="13" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1960,7 +1890,7 @@
       </c>
       <c r="J9" s="13"/>
       <c r="K9" s="14">
-        <v>0.35</v>
+        <v>0.25</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="12"/>
@@ -1975,7 +1905,7 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="13" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -2003,7 +1933,7 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="13" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -2072,7 +2002,7 @@
       </c>
       <c r="J13" s="13"/>
       <c r="K13" s="9">
-        <v>-0.65</v>
+        <v>-0.75</v>
       </c>
       <c r="L13" s="12"/>
       <c r="M13" s="11"/>
@@ -2149,406 +2079,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82BBA6E9-EE2B-41DB-98BC-F8BE2F6C02FF}">
-  <dimension ref="B1:AC15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-    </row>
-    <row r="2" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="X5" s="16"/>
-      <c r="Y5" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z5" s="16"/>
-      <c r="AA5" s="16"/>
-      <c r="AB5" s="16"/>
-      <c r="AC5" s="16"/>
-    </row>
-    <row r="6" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="13">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1">
-        <v>3</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="S6" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="X6" s="16"/>
-      <c r="Y6" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z6" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA6" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB6" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC6" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B7" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="13">
-        <v>2017</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1">
-        <v>0</v>
-      </c>
-      <c r="M7" s="1"/>
-      <c r="S7" t="s">
-        <v>47</v>
-      </c>
-      <c r="X7" s="18">
-        <v>2019</v>
-      </c>
-      <c r="Y7" s="17">
-        <v>4.4375644994840042E-2</v>
-      </c>
-      <c r="Z7" s="17">
-        <v>0.34416924664602683</v>
-      </c>
-      <c r="AA7" s="17">
-        <v>9.7523219814241488E-2</v>
-      </c>
-      <c r="AB7" s="17">
-        <v>0.51393188854489169</v>
-      </c>
-      <c r="AC7" s="18"/>
-    </row>
-    <row r="8" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B8" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1">
-        <v>0</v>
-      </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1">
-        <v>3</v>
-      </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="S8" t="s">
-        <v>31</v>
-      </c>
-      <c r="X8" s="18">
-        <v>2020</v>
-      </c>
-      <c r="Y8" s="17">
-        <v>2.8471818710052294E-2</v>
-      </c>
-      <c r="Z8" s="17">
-        <v>0.37943056362579897</v>
-      </c>
-      <c r="AA8" s="17">
-        <v>0.1167925624636839</v>
-      </c>
-      <c r="AB8" s="17">
-        <v>0.47530505520046484</v>
-      </c>
-      <c r="AC8" s="18"/>
-    </row>
-    <row r="9" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B9" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1">
-        <v>2030</v>
-      </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1">
-        <f>Y14</f>
-        <v>0.71578205413572371</v>
-      </c>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="X9" s="18">
-        <v>2021</v>
-      </c>
-      <c r="Y9" s="17">
-        <v>4.525455688246386E-2</v>
-      </c>
-      <c r="Z9" s="17">
-        <v>0.35575109993714643</v>
-      </c>
-      <c r="AA9" s="17">
-        <v>0.11816467630421119</v>
-      </c>
-      <c r="AB9" s="17">
-        <v>0.48082966687617851</v>
-      </c>
-      <c r="AC9" s="18"/>
-    </row>
-    <row r="10" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B10" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="1">
-        <v>0</v>
-      </c>
-      <c r="J10" s="13"/>
-      <c r="K10" s="1">
-        <v>3</v>
-      </c>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="X10" s="18">
-        <v>2022</v>
-      </c>
-      <c r="Y10" s="17">
-        <v>3.8644470868014272E-2</v>
-      </c>
-      <c r="Z10" s="17">
-        <v>0.38822829964328182</v>
-      </c>
-      <c r="AA10" s="17">
-        <v>4.1617122473246136E-2</v>
-      </c>
-      <c r="AB10" s="17">
-        <v>0.53151010701545776</v>
-      </c>
-      <c r="AC10" s="18"/>
-    </row>
-    <row r="11" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B11" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="1">
-        <v>2030</v>
-      </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="1">
-        <f>-1+K9</f>
-        <v>-0.28421794586427629</v>
-      </c>
-      <c r="L11" s="13"/>
-    </row>
-    <row r="12" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="13"/>
-      <c r="S12" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="L13" s="13"/>
-      <c r="S13" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="13"/>
-      <c r="S14" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y14">
-        <v>0.71578205413572371</v>
-      </c>
-    </row>
-    <row r="15" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="Y15">
-        <v>0.73042505592841167</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
P&P biomass cost update
Slight update on costs for biomass fuel for the boilers
</commit_message>
<xml_diff>
--- a/suppxls/Scen_UC_IND_IPP.xlsx
+++ b/suppxls/Scen_UC_IND_IPP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\CHP - Total Heat &amp; Power calibrattion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34B21B6-6CE7-4100-871A-495EF64EDDC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6F1E85-DB54-4388-8145-6541FBDD3B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35925" yWindow="3645" windowWidth="17280" windowHeight="8970" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UCT1" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="42">
   <si>
     <t>UC - Each Region/Period</t>
   </si>
@@ -147,9 +147,6 @@
   </si>
   <si>
     <t>Biomass consumed for piulping</t>
-  </si>
-  <si>
-    <t>IPPSTMBIO-E</t>
   </si>
 </sst>
 </file>
@@ -1669,7 +1666,7 @@
   <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1844,7 +1841,7 @@
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1877,7 +1874,7 @@
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1905,7 +1902,7 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1933,7 +1930,7 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>

</xml_diff>

<commit_message>
version of UC_IND_IPP that was in the last batch of NZ
</commit_message>
<xml_diff>
--- a/suppxls/Scen_UC_IND_IPP.xlsx
+++ b/suppxls/Scen_UC_IND_IPP.xlsx
@@ -5,23 +5,24 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\CHP - Total Heat &amp; Power calibrattion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6F1E85-DB54-4388-8145-6541FBDD3B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9786C1F-36F8-4689-92E8-BBFB0CA5C6BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UCT1" sheetId="2" r:id="rId1"/>
     <sheet name="UCT2" sheetId="3" r:id="rId2"/>
+    <sheet name="UCT4" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="58">
   <si>
     <t>UC - Each Region/Period</t>
   </si>
@@ -147,6 +148,54 @@
   </si>
   <si>
     <t>Biomass consumed for piulping</t>
+  </si>
+  <si>
+    <t>UCACT_IPP_CHP</t>
+  </si>
+  <si>
+    <t>Set max fossil fuel (FF) share to renewable (RE) fuel utilisation ratio</t>
+  </si>
+  <si>
+    <t>Dissolving pulp</t>
+  </si>
+  <si>
+    <t>Chemical pulping</t>
+  </si>
+  <si>
+    <t>IPPCHE_N</t>
+  </si>
+  <si>
+    <t>IPPDIS_E</t>
+  </si>
+  <si>
+    <t>LO</t>
+  </si>
+  <si>
+    <t>Market shares</t>
+  </si>
+  <si>
+    <t>Mechanical Pulp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chemical Pulp </t>
+  </si>
+  <si>
+    <t>Semi-chemical Pulp</t>
+  </si>
+  <si>
+    <t>Dissolving wood Pulp</t>
+  </si>
+  <si>
+    <t>Total Pulp</t>
+  </si>
+  <si>
+    <t>Min ratio of DIS to Che pulping</t>
+  </si>
+  <si>
+    <t>IPPDIS-N, IPPDIS-E</t>
+  </si>
+  <si>
+    <t>IPPCHE-N, IPPCHE-E</t>
   </si>
 </sst>
 </file>
@@ -160,7 +209,7 @@
     <numFmt numFmtId="166" formatCode="[$£-809]#,##0.000;[Red]&quot;-&quot;[$£-809]#,##0.000"/>
     <numFmt numFmtId="167" formatCode="[$£-809]#,##0.00;[Red]&quot;-&quot;[$£-809]#,##0.00"/>
   </numFmts>
-  <fonts count="38" x14ac:knownFonts="1">
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,7 +352,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -392,6 +440,13 @@
       <color theme="6" tint="-0.24994659260841701"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -519,7 +574,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -572,6 +627,21 @@
       <top/>
       <bottom style="thick">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -759,11 +829,11 @@
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="167" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="4" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="4" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -774,7 +844,7 @@
     <xf numFmtId="167" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="167" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -795,6 +865,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="36" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="178">
     <cellStyle name="20% - Accent1 2" xfId="17" xr:uid="{03071494-95FB-4D44-BFD8-23D5C5460AB0}"/>
@@ -1307,7 +1380,7 @@
   <dimension ref="B1:S18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1666,7 +1739,7 @@
   <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1887,7 +1960,7 @@
       </c>
       <c r="J9" s="13"/>
       <c r="K9" s="14">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="12"/>
@@ -1999,7 +2072,7 @@
       </c>
       <c r="J13" s="13"/>
       <c r="K13" s="9">
-        <v>-0.75</v>
+        <v>-0.65</v>
       </c>
       <c r="L13" s="12"/>
       <c r="M13" s="11"/>
@@ -2076,4 +2149,406 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82BBA6E9-EE2B-41DB-98BC-F8BE2F6C02FF}">
+  <dimension ref="B1:AC15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z5" s="16"/>
+      <c r="AA5" s="16"/>
+      <c r="AB5" s="16"/>
+      <c r="AC5" s="16"/>
+    </row>
+    <row r="6" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B6" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="13">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1">
+        <v>3</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z6" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA6" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB6" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC6" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B7" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="13">
+        <v>2017</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1"/>
+      <c r="S7" t="s">
+        <v>47</v>
+      </c>
+      <c r="X7" s="18">
+        <v>2019</v>
+      </c>
+      <c r="Y7" s="17">
+        <v>4.4375644994840042E-2</v>
+      </c>
+      <c r="Z7" s="17">
+        <v>0.34416924664602683</v>
+      </c>
+      <c r="AA7" s="17">
+        <v>9.7523219814241488E-2</v>
+      </c>
+      <c r="AB7" s="17">
+        <v>0.51393188854489169</v>
+      </c>
+      <c r="AC7" s="18"/>
+    </row>
+    <row r="8" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B8" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1">
+        <v>3</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="S8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X8" s="18">
+        <v>2020</v>
+      </c>
+      <c r="Y8" s="17">
+        <v>2.8471818710052294E-2</v>
+      </c>
+      <c r="Z8" s="17">
+        <v>0.37943056362579897</v>
+      </c>
+      <c r="AA8" s="17">
+        <v>0.1167925624636839</v>
+      </c>
+      <c r="AB8" s="17">
+        <v>0.47530505520046484</v>
+      </c>
+      <c r="AC8" s="18"/>
+    </row>
+    <row r="9" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B9" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1">
+        <v>2030</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1">
+        <f>Y14</f>
+        <v>0.71578205413572371</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="X9" s="18">
+        <v>2021</v>
+      </c>
+      <c r="Y9" s="17">
+        <v>4.525455688246386E-2</v>
+      </c>
+      <c r="Z9" s="17">
+        <v>0.35575109993714643</v>
+      </c>
+      <c r="AA9" s="17">
+        <v>0.11816467630421119</v>
+      </c>
+      <c r="AB9" s="17">
+        <v>0.48082966687617851</v>
+      </c>
+      <c r="AC9" s="18"/>
+    </row>
+    <row r="10" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B10" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="13"/>
+      <c r="K10" s="1">
+        <v>3</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="X10" s="18">
+        <v>2022</v>
+      </c>
+      <c r="Y10" s="17">
+        <v>3.8644470868014272E-2</v>
+      </c>
+      <c r="Z10" s="17">
+        <v>0.38822829964328182</v>
+      </c>
+      <c r="AA10" s="17">
+        <v>4.1617122473246136E-2</v>
+      </c>
+      <c r="AB10" s="17">
+        <v>0.53151010701545776</v>
+      </c>
+      <c r="AC10" s="18"/>
+    </row>
+    <row r="11" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B11" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="1">
+        <v>2030</v>
+      </c>
+      <c r="J11" s="13"/>
+      <c r="K11" s="1">
+        <f>-1+K9</f>
+        <v>-0.28421794586427629</v>
+      </c>
+      <c r="L11" s="13"/>
+    </row>
+    <row r="12" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="13"/>
+      <c r="S12" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="L13" s="13"/>
+      <c r="S13" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="13"/>
+      <c r="S14" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y14">
+        <v>0.71578205413572371</v>
+      </c>
+    </row>
+    <row r="15" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="Y15">
+        <v>0.73042505592841167</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
2nd Attempt for restoring UC_IND_IPP
</commit_message>
<xml_diff>
--- a/suppxls/Scen_UC_IND_IPP.xlsx
+++ b/suppxls/Scen_UC_IND_IPP.xlsx
@@ -2,22 +2,35 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9786C1F-36F8-4689-92E8-BBFB0CA5C6BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C5C61D-BFCD-49E6-86B9-2BC4C6041FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3540" yWindow="-18240" windowWidth="24630" windowHeight="15330" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UCT1" sheetId="2" r:id="rId1"/>
     <sheet name="UCT2" sheetId="3" r:id="rId2"/>
     <sheet name="UCT4" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -150,9 +163,6 @@
     <t>Biomass consumed for piulping</t>
   </si>
   <si>
-    <t>UCACT_IPP_CHP</t>
-  </si>
-  <si>
     <t>Set max fossil fuel (FF) share to renewable (RE) fuel utilisation ratio</t>
   </si>
   <si>
@@ -196,6 +206,9 @@
   </si>
   <si>
     <t>IPPCHE-N, IPPCHE-E</t>
+  </si>
+  <si>
+    <t>UCACT_IPP_PULP</t>
   </si>
 </sst>
 </file>
@@ -203,8 +216,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="166" formatCode="[$£-809]#,##0.000;[Red]&quot;-&quot;[$£-809]#,##0.000"/>
     <numFmt numFmtId="167" formatCode="[$£-809]#,##0.00;[Red]&quot;-&quot;[$£-809]#,##0.00"/>
@@ -352,6 +365,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -663,7 +677,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -673,13 +687,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -689,18 +703,18 @@
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -725,19 +739,19 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -748,47 +762,47 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="32" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -796,7 +810,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -825,9 +839,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="167" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="4" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="center"/>
@@ -1377,15 +1391,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B12370F-117E-47ED-B36F-AF074D2BFFD5}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:S18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1402,7 +1417,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1418,7 +1433,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1434,7 +1449,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1450,7 +1465,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1488,7 +1503,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>16</v>
       </c>
@@ -1514,7 +1529,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>16</v>
       </c>
@@ -1535,7 +1550,7 @@
       </c>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>16</v>
       </c>
@@ -1563,7 +1578,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>16</v>
       </c>
@@ -1588,7 +1603,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>16</v>
       </c>
@@ -1610,7 +1625,7 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>16</v>
       </c>
@@ -1631,7 +1646,7 @@
       </c>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>16</v>
       </c>
@@ -1648,7 +1663,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -1665,7 +1680,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>16</v>
       </c>
@@ -1685,7 +1700,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>16</v>
       </c>
@@ -1705,7 +1720,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="O16" t="s">
         <v>30</v>
       </c>
@@ -1713,7 +1728,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="15:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="15:19" x14ac:dyDescent="0.25">
       <c r="O17" t="s">
         <v>32</v>
       </c>
@@ -1721,7 +1736,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="15:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="15:19" x14ac:dyDescent="0.25">
       <c r="O18" t="s">
         <v>23</v>
       </c>
@@ -1736,19 +1751,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A9D59EF-94E7-45A0-A820-0537C3C9B3DC}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="32.21875" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1764,7 +1780,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1780,7 +1796,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1796,7 +1812,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1812,7 +1828,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1850,7 +1866,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="13" t="s">
         <v>35</v>
@@ -1882,7 +1898,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
         <v>35</v>
       </c>
@@ -1908,7 +1924,7 @@
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
         <v>35</v>
       </c>
@@ -1941,7 +1957,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
         <v>35</v>
       </c>
@@ -1969,7 +1985,7 @@
       <c r="P9" s="11"/>
       <c r="Q9" s="11"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
         <v>35</v>
       </c>
@@ -1997,7 +2013,7 @@
       <c r="P10" s="11"/>
       <c r="Q10" s="11"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B11" s="13" t="s">
         <v>35</v>
       </c>
@@ -2025,7 +2041,7 @@
       <c r="P11" s="11"/>
       <c r="Q11" s="11"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B12" s="13" t="s">
         <v>35</v>
       </c>
@@ -2053,7 +2069,7 @@
       <c r="P12" s="11"/>
       <c r="Q12" s="11"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
         <v>35</v>
       </c>
@@ -2081,7 +2097,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B14" s="13" t="s">
         <v>35</v>
       </c>
@@ -2109,7 +2125,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B15" s="13" t="s">
         <v>35</v>
       </c>
@@ -2134,7 +2150,7 @@
       <c r="M15" s="11"/>
       <c r="N15" s="11"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
@@ -2153,15 +2169,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82BBA6E9-EE2B-41DB-98BC-F8BE2F6C02FF}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:AC15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2177,7 +2194,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2193,7 +2210,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2209,7 +2226,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -2225,7 +2242,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
@@ -2264,16 +2281,16 @@
       </c>
       <c r="X5" s="16"/>
       <c r="Y5" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Z5" s="16"/>
       <c r="AA5" s="16"/>
       <c r="AB5" s="16"/>
       <c r="AC5" s="16"/>
     </row>
-    <row r="6" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="13"/>
@@ -2285,38 +2302,38 @@
         <v>0</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1">
         <v>3</v>
       </c>
       <c r="M6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S6" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="S6" s="8" t="s">
-        <v>44</v>
       </c>
       <c r="X6" s="16"/>
       <c r="Y6" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z6" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="Z6" s="18" t="s">
+      <c r="AA6" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="AA6" s="18" t="s">
+      <c r="AB6" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="AB6" s="18" t="s">
+      <c r="AC6" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AC6" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="2:29" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="13"/>
@@ -2328,7 +2345,7 @@
         <v>2017</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1">
@@ -2336,7 +2353,7 @@
       </c>
       <c r="M7" s="1"/>
       <c r="S7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="X7" s="18">
         <v>2019</v>
@@ -2355,13 +2372,13 @@
       </c>
       <c r="AC7" s="18"/>
     </row>
-    <row r="8" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -2396,13 +2413,13 @@
       </c>
       <c r="AC8" s="18"/>
     </row>
-    <row r="9" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -2435,13 +2452,13 @@
       </c>
       <c r="AC9" s="18"/>
     </row>
-    <row r="10" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
@@ -2473,13 +2490,13 @@
       </c>
       <c r="AC10" s="18"/>
     </row>
-    <row r="11" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B11" s="13" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
@@ -2495,7 +2512,7 @@
       </c>
       <c r="L11" s="13"/>
     </row>
-    <row r="12" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -2508,19 +2525,19 @@
       <c r="K12" s="1"/>
       <c r="L12" s="13"/>
       <c r="S12" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="2:29" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="2:29" x14ac:dyDescent="0.25">
       <c r="L13" s="13"/>
       <c r="S13" t="s">
         <v>27</v>
       </c>
       <c r="Y13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="2:29" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -2533,13 +2550,13 @@
       <c r="K14" s="1"/>
       <c r="L14" s="13"/>
       <c r="S14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Y14">
         <v>0.71578205413572371</v>
       </c>
     </row>
-    <row r="15" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>

</xml_diff>